<commit_message>
Updated DataScience Life Cycle Sheet
</commit_message>
<xml_diff>
--- a/DataScience-LifeCycle.xlsx
+++ b/DataScience-LifeCycle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sudhanshu\gitrepository\Data-Science-Projects\Real-Estate-Price-Prediction-Model-with-NLP-and-FastAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35930046-57AD-4D2A-8DB3-2B1971B952C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C931D22-CFA0-4705-8618-87181ADCA5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>S.No</t>
   </si>
@@ -38,12 +38,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
   </si>
   <si>
     <t>Data Loading</t>
@@ -85,9 +79,6 @@
   </si>
   <si>
     <t>Two Way ANOVA</t>
-  </si>
-  <si>
-    <t>Not Applicable</t>
   </si>
   <si>
     <t>Data Preparation</t>
@@ -166,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -190,10 +181,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -205,39 +196,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -281,17 +241,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -325,34 +274,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -360,79 +294,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -715,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,11 +632,10 @@
     <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.42578125" customWidth="1"/>
+    <col min="6" max="6" width="64.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,325 +649,246 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="31" t="s">
+      <c r="E2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>4</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="11">
-        <v>45139</v>
-      </c>
-      <c r="G2" s="12">
-        <v>45139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="48" t="s">
+      <c r="E7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>5</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="13">
-        <v>45139</v>
-      </c>
-      <c r="G3" s="14">
-        <v>45139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="44" t="s">
+      <c r="E17" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4">
-        <v>45141</v>
-      </c>
-      <c r="G4" s="5">
-        <v>45142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="30" t="s">
+      <c r="E18" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4">
-        <v>45141</v>
-      </c>
-      <c r="G5" s="5">
-        <v>45142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="6">
-        <v>45141</v>
-      </c>
-      <c r="G6" s="7">
-        <v>45142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
-        <v>4</v>
-      </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="24">
-        <v>45142</v>
-      </c>
-      <c r="G7" s="3">
-        <v>45143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="25">
-        <v>45142</v>
-      </c>
-      <c r="G8" s="5">
-        <v>45143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="26">
-        <v>45142</v>
-      </c>
-      <c r="G9" s="7">
-        <v>45143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
-        <v>5</v>
-      </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="33"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="27">
-        <v>45144</v>
-      </c>
-      <c r="G13" s="27">
-        <v>45144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="27">
-        <v>45144</v>
-      </c>
-      <c r="G15" s="28">
-        <v>45144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
-        <v>6</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="19"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="19"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="7"/>
+      <c r="E20" s="10" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="B16:B20"/>
     <mergeCell ref="B3:B15"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="C13:C15"/>
-    <mergeCell ref="F10:G12"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="C16:C20"/>
     <mergeCell ref="C4:C6"/>
@@ -1091,7 +916,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>